<commit_message>
cleaned up code and added comments for mentors and project requirements
</commit_message>
<xml_diff>
--- a/LEGO search results September 28, 2021.xlsx
+++ b/LEGO search results September 28, 2021.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="77">
   <si>
     <t>LEGO Set Name</t>
   </si>
@@ -52,15 +52,15 @@
     <t>Hogwarts™ Moment: Herbology Class</t>
   </si>
   <si>
+    <t>Hogwarts™ Whomping Willow™</t>
+  </si>
+  <si>
+    <t>Hogwarts™ Room of Requirement</t>
+  </si>
+  <si>
     <t>Hagrid's Hut: Buckbeak's Rescue</t>
   </si>
   <si>
-    <t>Hogwarts™ Whomping Willow™</t>
-  </si>
-  <si>
-    <t>Hogwarts™ Room of Requirement</t>
-  </si>
-  <si>
     <t>Attack on the Burrow</t>
   </si>
   <si>
@@ -70,54 +70,54 @@
     <t>Forbidden Forest: Umbridge's Encounter</t>
   </si>
   <si>
+    <t>Hogwarts™ Moment: Potions Class</t>
+  </si>
+  <si>
     <t>Hogwarts™ Students Acc. Set</t>
   </si>
   <si>
     <t>Voldemort™, Nagini &amp; Bellatrix</t>
   </si>
   <si>
+    <t>Hogwarts™ Wizard’s Chess</t>
+  </si>
+  <si>
     <t>Harry Potter™ Key Chain</t>
   </si>
   <si>
-    <t>Hogwarts™ Wizard’s Chess</t>
-  </si>
-  <si>
     <t>Harry Potter™ Hogwarts™ Crests</t>
   </si>
   <si>
+    <t>Hogwarts™: Polyjuice Potion Mistake</t>
+  </si>
+  <si>
     <t>Hogwarts™ Icons - Collectors' Edition</t>
   </si>
   <si>
-    <t>Hogwarts™ Moment: Potions Class</t>
-  </si>
-  <si>
     <t>The Knight Bus™</t>
   </si>
   <si>
     <t>Hogwarts™ Moment: Charms Class</t>
   </si>
   <si>
-    <t>Hogwarts™: Polyjuice Potion Mistake</t>
+    <t>Hogwarts™: First Flying Lesson</t>
   </si>
   <si>
     <t>Hogwarts™ Moment: Transfiguration Class</t>
   </si>
   <si>
-    <t>Hogwarts™: First Flying Lesson</t>
-  </si>
-  <si>
     <t>Hogwarts™ Chamber of Secrets</t>
   </si>
   <si>
+    <t>Hogwarts™: Fluffy Encounter</t>
+  </si>
+  <si>
+    <t>Hogsmeade™ Village Visit</t>
+  </si>
+  <si>
     <t>Diagon Alley™</t>
   </si>
   <si>
-    <t>Hogwarts™: Fluffy Encounter</t>
-  </si>
-  <si>
-    <t>Hogsmeade™ Village Visit</t>
-  </si>
-  <si>
     <t>Fawkes, Dumbledore’s Phoenix</t>
   </si>
   <si>
@@ -127,15 +127,18 @@
     <t>Ron Key Chain</t>
   </si>
   <si>
+    <t>The Rise of Voldemort™</t>
+  </si>
+  <si>
+    <t>Harry Potter™ &amp; Hedwig™</t>
+  </si>
+  <si>
+    <t>Harry Potter™ and Fantastic Beasts™</t>
+  </si>
+  <si>
     <t>Hogwarts™ Great Hall</t>
   </si>
   <si>
-    <t>Harry Potter™ and Fantastic Beasts™</t>
-  </si>
-  <si>
-    <t>Harry Potter™ &amp; Hedwig™</t>
-  </si>
-  <si>
     <t>Beauxbatons’ Carriage: Arrival at Hogwarts™</t>
   </si>
   <si>
@@ -205,10 +208,10 @@
     <t>$29.99</t>
   </si>
   <si>
+    <t>$19.99</t>
+  </si>
+  <si>
     <t>$59.99</t>
-  </si>
-  <si>
-    <t>$19.99</t>
   </si>
   <si>
     <t>$79.99</t>
@@ -604,10 +607,10 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -615,10 +618,10 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -626,10 +629,10 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -637,10 +640,10 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -648,10 +651,10 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C6" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -659,10 +662,10 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C7" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -670,10 +673,10 @@
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C8" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -681,10 +684,10 @@
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C9" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -692,10 +695,10 @@
         <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C10" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -703,10 +706,10 @@
         <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C11" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -714,10 +717,10 @@
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="C12" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -725,10 +728,10 @@
         <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C13" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -736,10 +739,10 @@
         <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C14" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -747,10 +750,10 @@
         <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C15" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -758,10 +761,10 @@
         <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C16" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -769,10 +772,10 @@
         <v>18</v>
       </c>
       <c r="B17" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C17" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -780,10 +783,10 @@
         <v>19</v>
       </c>
       <c r="B18" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="C18" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -791,10 +794,10 @@
         <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C19" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -802,10 +805,10 @@
         <v>21</v>
       </c>
       <c r="B20" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C20" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -813,10 +816,10 @@
         <v>22</v>
       </c>
       <c r="B21" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="C21" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -824,10 +827,10 @@
         <v>23</v>
       </c>
       <c r="B22" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C22" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -835,10 +838,10 @@
         <v>24</v>
       </c>
       <c r="B23" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C23" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -846,10 +849,10 @@
         <v>25</v>
       </c>
       <c r="B24" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="C24" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -857,10 +860,10 @@
         <v>26</v>
       </c>
       <c r="B25" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C25" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -868,10 +871,10 @@
         <v>27</v>
       </c>
       <c r="B26" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C26" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -879,10 +882,10 @@
         <v>28</v>
       </c>
       <c r="B27" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C27" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -890,10 +893,10 @@
         <v>29</v>
       </c>
       <c r="B28" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C28" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -901,10 +904,10 @@
         <v>30</v>
       </c>
       <c r="B29" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C29" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -912,10 +915,10 @@
         <v>31</v>
       </c>
       <c r="B30" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="C30" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -923,10 +926,10 @@
         <v>32</v>
       </c>
       <c r="B31" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="C31" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -934,10 +937,10 @@
         <v>33</v>
       </c>
       <c r="B32" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="C32" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -945,10 +948,10 @@
         <v>34</v>
       </c>
       <c r="B33" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C33" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -956,10 +959,10 @@
         <v>35</v>
       </c>
       <c r="B34" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C34" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -967,10 +970,10 @@
         <v>36</v>
       </c>
       <c r="B35" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C35" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -978,10 +981,10 @@
         <v>7</v>
       </c>
       <c r="B36" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C36" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -989,7 +992,7 @@
         <v>37</v>
       </c>
       <c r="B37" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="C37" t="s">
         <v>75</v>
@@ -997,10 +1000,10 @@
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B38" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="C38" t="s">
         <v>75</v>
@@ -1008,200 +1011,200 @@
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B39" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C39" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B40" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C40" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B41" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C41" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B42" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C42" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B43" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C43" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B44" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C44" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B45" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C45" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B46" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C46" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B47" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C47" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B48" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C48" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B49" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C49" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B50" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C50" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B51" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C51" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B52" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C52" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B53" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C53" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B54" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C54" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B55" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C55" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C56" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>